<commit_message>
added commands to button
</commit_message>
<xml_diff>
--- a/cache/all.xlsx
+++ b/cache/all.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="108" windowWidth="16212" windowHeight="5808"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="25">
   <si>
     <t>id</t>
   </si>
@@ -40,6 +40,9 @@
     <t>times_repaired</t>
   </si>
   <si>
+    <t>pay_for_repair</t>
+  </si>
+  <si>
     <t>gain</t>
   </si>
   <si>
@@ -49,7 +52,19 @@
     <t>rented_time</t>
   </si>
   <si>
-    <t>mili_meter_reading_on_rent</t>
+    <t>milli_meter_reading_on_rent</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>advance</t>
+  </si>
+  <si>
+    <t>per_hour</t>
+  </si>
+  <si>
+    <t>per_km</t>
   </si>
   <si>
     <t>Honda City</t>
@@ -59,12 +74,6 @@
   </si>
   <si>
     <t>yes</t>
-  </si>
-  <si>
-    <t>pay_for_repair</t>
-  </si>
-  <si>
-    <t>AC</t>
   </si>
   <si>
     <t>Tata Sumo</t>
@@ -79,7 +88,7 @@
     <t>Mahindra Bolero</t>
   </si>
   <si>
-    <t>advance</t>
+    <t>new</t>
   </si>
 </sst>
 </file>
@@ -411,22 +420,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O53"/>
+  <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="2" max="2" width="10.77734375" customWidth="1"/>
-    <col min="7" max="8" width="12.77734375" customWidth="1"/>
-    <col min="9" max="9" width="15.77734375" customWidth="1"/>
-    <col min="11" max="12" width="12.77734375" customWidth="1"/>
-    <col min="13" max="13" width="30.77734375" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -452,42 +452,48 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="O1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F2">
         <v>1000000</v>
@@ -514,27 +520,33 @@
         <v>0</v>
       </c>
       <c r="N2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:15">
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F3">
         <v>1000000</v>
@@ -561,27 +573,33 @@
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:15">
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F4">
         <v>1000000</v>
@@ -608,27 +626,33 @@
         <v>0</v>
       </c>
       <c r="N4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:15">
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F5">
         <v>1000000</v>
@@ -655,27 +679,33 @@
         <v>0</v>
       </c>
       <c r="N5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:15">
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F6">
         <v>1000000</v>
@@ -702,27 +732,33 @@
         <v>0</v>
       </c>
       <c r="N6" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:15">
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F7">
         <v>1000000</v>
@@ -749,27 +785,33 @@
         <v>0</v>
       </c>
       <c r="N7" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:15">
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F8">
         <v>1000000</v>
@@ -796,27 +838,33 @@
         <v>0</v>
       </c>
       <c r="N8" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:15">
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F9">
         <v>1000000</v>
@@ -843,27 +891,33 @@
         <v>0</v>
       </c>
       <c r="N9" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F10">
         <v>1000000</v>
@@ -890,27 +944,33 @@
         <v>0</v>
       </c>
       <c r="N10" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F11">
         <v>1000000</v>
@@ -937,27 +997,33 @@
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E12" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F12">
         <v>1000000</v>
@@ -984,27 +1050,33 @@
         <v>0</v>
       </c>
       <c r="N12" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:15">
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E13" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F13">
         <v>1000000</v>
@@ -1031,27 +1103,33 @@
         <v>0</v>
       </c>
       <c r="N13" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="O13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:15">
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E14" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F14">
         <v>1000000</v>
@@ -1078,27 +1156,33 @@
         <v>0</v>
       </c>
       <c r="N14" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:15">
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E15" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F15">
         <v>1000000</v>
@@ -1125,27 +1209,33 @@
         <v>0</v>
       </c>
       <c r="N15" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:15">
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E16" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F16">
         <v>1000000</v>
@@ -1172,27 +1262,33 @@
         <v>0</v>
       </c>
       <c r="N16" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="O16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:15">
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E17" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F17">
         <v>1000000</v>
@@ -1219,27 +1315,33 @@
         <v>0</v>
       </c>
       <c r="N17" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="O17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:15">
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E18" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F18">
         <v>1000000</v>
@@ -1266,27 +1368,33 @@
         <v>0</v>
       </c>
       <c r="N18" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="O18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:15">
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F19">
         <v>1000000</v>
@@ -1313,27 +1421,33 @@
         <v>0</v>
       </c>
       <c r="N19" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:15">
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E20" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F20">
         <v>1000000</v>
@@ -1360,27 +1474,33 @@
         <v>0</v>
       </c>
       <c r="N20" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:15">
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E21" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F21">
         <v>1000000</v>
@@ -1407,27 +1527,33 @@
         <v>0</v>
       </c>
       <c r="N21" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:15">
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D22" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E22" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F22">
         <v>1000000</v>
@@ -1454,27 +1580,33 @@
         <v>0</v>
       </c>
       <c r="N22" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:15">
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D23" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E23" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F23">
         <v>1000000</v>
@@ -1501,27 +1633,33 @@
         <v>0</v>
       </c>
       <c r="N23" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:15">
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C24" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E24" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F24">
         <v>1000000</v>
@@ -1548,27 +1686,33 @@
         <v>0</v>
       </c>
       <c r="N24" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:15">
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D25" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E25" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F25">
         <v>1000000</v>
@@ -1595,27 +1739,33 @@
         <v>0</v>
       </c>
       <c r="N25" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:15">
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C26" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D26" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E26" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F26">
         <v>1000000</v>
@@ -1642,27 +1792,33 @@
         <v>0</v>
       </c>
       <c r="N26" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:15">
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C27" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D27" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E27" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F27">
         <v>1000000</v>
@@ -1689,27 +1845,33 @@
         <v>0</v>
       </c>
       <c r="N27" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:15">
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C28" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D28" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E28" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F28">
         <v>1000000</v>
@@ -1736,27 +1898,33 @@
         <v>0</v>
       </c>
       <c r="N28" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:15">
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C29" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D29" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E29" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F29">
         <v>1000000</v>
@@ -1783,27 +1951,33 @@
         <v>0</v>
       </c>
       <c r="N29" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:15">
+      <c r="P29">
+        <v>0</v>
+      </c>
+      <c r="Q29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C30" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D30" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E30" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F30">
         <v>1000000</v>
@@ -1830,27 +2004,33 @@
         <v>0</v>
       </c>
       <c r="N30" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:15">
+      <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C31" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D31" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E31" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F31">
         <v>1000000</v>
@@ -1877,27 +2057,33 @@
         <v>0</v>
       </c>
       <c r="N31" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:15">
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C32" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D32" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E32" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F32">
         <v>1000000</v>
@@ -1924,27 +2110,33 @@
         <v>0</v>
       </c>
       <c r="N32" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:15">
+      <c r="P32">
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C33" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D33" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E33" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F33">
         <v>1000000</v>
@@ -1971,27 +2163,33 @@
         <v>0</v>
       </c>
       <c r="N33" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:15">
+      <c r="P33">
+        <v>0</v>
+      </c>
+      <c r="Q33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C34" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D34" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E34" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F34">
         <v>1000000</v>
@@ -2018,27 +2216,33 @@
         <v>0</v>
       </c>
       <c r="N34" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="O34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:15">
+      <c r="P34">
+        <v>0</v>
+      </c>
+      <c r="Q34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C35" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D35" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E35" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F35">
         <v>1000000</v>
@@ -2065,27 +2269,33 @@
         <v>0</v>
       </c>
       <c r="N35" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="O35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:15">
+      <c r="P35">
+        <v>0</v>
+      </c>
+      <c r="Q35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C36" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D36" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E36" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F36">
         <v>1000000</v>
@@ -2112,27 +2322,33 @@
         <v>0</v>
       </c>
       <c r="N36" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="O36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:15">
+      <c r="P36">
+        <v>0</v>
+      </c>
+      <c r="Q36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C37" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D37" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E37" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F37">
         <v>1000000</v>
@@ -2159,27 +2375,33 @@
         <v>0</v>
       </c>
       <c r="N37" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="O37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:15">
+      <c r="P37">
+        <v>0</v>
+      </c>
+      <c r="Q37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C38" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D38" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E38" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F38">
         <v>1000000</v>
@@ -2206,27 +2428,33 @@
         <v>0</v>
       </c>
       <c r="N38" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="O38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:15">
+      <c r="P38">
+        <v>0</v>
+      </c>
+      <c r="Q38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C39" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D39" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E39" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F39">
         <v>1000000</v>
@@ -2253,27 +2481,33 @@
         <v>0</v>
       </c>
       <c r="N39" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="O39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:15">
+      <c r="P39">
+        <v>0</v>
+      </c>
+      <c r="Q39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C40" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D40" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E40" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F40">
         <v>1000000</v>
@@ -2300,27 +2534,33 @@
         <v>0</v>
       </c>
       <c r="N40" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="O40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:15">
+      <c r="P40">
+        <v>0</v>
+      </c>
+      <c r="Q40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C41" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D41" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E41" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F41">
         <v>1000000</v>
@@ -2347,27 +2587,33 @@
         <v>0</v>
       </c>
       <c r="N41" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="O41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:15">
+      <c r="P41">
+        <v>0</v>
+      </c>
+      <c r="Q41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C42" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D42" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E42" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F42">
         <v>1000000</v>
@@ -2394,27 +2640,33 @@
         <v>0</v>
       </c>
       <c r="N42" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="O42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:15">
+      <c r="P42">
+        <v>0</v>
+      </c>
+      <c r="Q42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C43" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D43" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E43" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F43">
         <v>1000000</v>
@@ -2441,27 +2693,33 @@
         <v>0</v>
       </c>
       <c r="N43" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="O43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:15">
+      <c r="P43">
+        <v>0</v>
+      </c>
+      <c r="Q43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C44" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D44" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E44" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F44">
         <v>1000000</v>
@@ -2488,27 +2746,33 @@
         <v>0</v>
       </c>
       <c r="N44" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:15">
+      <c r="P44">
+        <v>0</v>
+      </c>
+      <c r="Q44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C45" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D45" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E45" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F45">
         <v>1000000</v>
@@ -2535,27 +2799,33 @@
         <v>0</v>
       </c>
       <c r="N45" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:15">
+      <c r="P45">
+        <v>0</v>
+      </c>
+      <c r="Q45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C46" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D46" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E46" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F46">
         <v>1000000</v>
@@ -2582,27 +2852,33 @@
         <v>0</v>
       </c>
       <c r="N46" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:15">
+      <c r="P46">
+        <v>0</v>
+      </c>
+      <c r="Q46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C47" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D47" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E47" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F47">
         <v>1000000</v>
@@ -2629,27 +2905,33 @@
         <v>0</v>
       </c>
       <c r="N47" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:15">
+      <c r="P47">
+        <v>0</v>
+      </c>
+      <c r="Q47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C48" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D48" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E48" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F48">
         <v>1000000</v>
@@ -2676,27 +2958,33 @@
         <v>0</v>
       </c>
       <c r="N48" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:15">
+      <c r="P48">
+        <v>0</v>
+      </c>
+      <c r="Q48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C49" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D49" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E49" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F49">
         <v>1000000</v>
@@ -2723,27 +3011,33 @@
         <v>0</v>
       </c>
       <c r="N49" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:15">
+      <c r="P49">
+        <v>0</v>
+      </c>
+      <c r="Q49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C50" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D50" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E50" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F50">
         <v>1000000</v>
@@ -2770,27 +3064,33 @@
         <v>0</v>
       </c>
       <c r="N50" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:15">
+      <c r="P50">
+        <v>0</v>
+      </c>
+      <c r="Q50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C51" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D51" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E51" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F51">
         <v>1000000</v>
@@ -2817,27 +3117,33 @@
         <v>0</v>
       </c>
       <c r="N51" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:15">
+      <c r="P51">
+        <v>0</v>
+      </c>
+      <c r="Q51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C52" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D52" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E52" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F52">
         <v>1000000</v>
@@ -2864,27 +3170,33 @@
         <v>0</v>
       </c>
       <c r="N52" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:15">
+      <c r="P52">
+        <v>0</v>
+      </c>
+      <c r="Q52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C53" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D53" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E53" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F53">
         <v>1000000</v>
@@ -2911,10 +3223,69 @@
         <v>0</v>
       </c>
       <c r="N53" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="O53">
         <v>0</v>
+      </c>
+      <c r="P53">
+        <v>0</v>
+      </c>
+      <c r="Q53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>24</v>
+      </c>
+      <c r="C54" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54" t="s">
+        <v>18</v>
+      </c>
+      <c r="E54" t="s">
+        <v>19</v>
+      </c>
+      <c r="F54">
+        <v>200</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <v>0</v>
+      </c>
+      <c r="L54">
+        <v>0</v>
+      </c>
+      <c r="M54">
+        <v>0</v>
+      </c>
+      <c r="N54" t="s">
+        <v>19</v>
+      </c>
+      <c r="O54">
+        <v>0</v>
+      </c>
+      <c r="P54">
+        <v>200</v>
+      </c>
+      <c r="Q54">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>